<commit_message>
Updated powerpoint, add text to each figure, add filter to bar chart, gantt chart, re-vamp code for gantt chart to fix order, spacing, start/stop dates
</commit_message>
<xml_diff>
--- a/template_project_tracker.xlsx
+++ b/template_project_tracker.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Biostats\R\proj_mgmnt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B61424-326F-4CB7-BC87-5CDD8E007399}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9BCC5B-868A-41E2-BE19-285ADC3C390A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{FB338184-5F84-4174-A6E6-8D94051AC255}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hours Tracker" sheetId="1" r:id="rId1"/>
+    <sheet name="Project Tracker" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -45,12 +49,60 @@
   </si>
   <si>
     <t>Project phase</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Study title</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Current status</t>
+  </si>
+  <si>
+    <t>As of</t>
+  </si>
+  <si>
+    <t>Project initiated</t>
+  </si>
+  <si>
+    <t>Project completed</t>
+  </si>
+  <si>
+    <t>Final product</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>Manuscript</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Re-analysis</t>
+  </si>
+  <si>
+    <t>Sample Project</t>
+  </si>
+  <si>
+    <t>Last, First</t>
+  </si>
+  <si>
+    <t>Survival analyses in progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mmm\-dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,12 +120,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -97,10 +155,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -116,6 +190,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hours tracker"/>
+      <sheetName val="Project tracker"/>
+      <sheetName val="Completed"/>
+      <sheetName val="Vacation Days 2019"/>
+      <sheetName val="Vacation Days 2020"/>
+      <sheetName val="Abstracts"/>
+      <sheetName val="Vacation Days 2018"/>
+      <sheetName val="Vacation Days 2017"/>
+      <sheetName val="Sheet 1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,14 +521,14 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
@@ -448,7 +551,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2">
+        <v>43880</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -468,4 +585,87 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E7D888-5A5F-4200-B8B0-57E569E37EC6}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="8">
+        <v>43857</v>
+      </c>
+      <c r="F2" s="9">
+        <v>42817</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="7">
+        <f>SUMIF('Hours Tracker'!C:C, 'Project Tracker'!B2, 'Hours Tracker'!B:B)</f>
+        <v>3</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>